<commit_message>
updated parameters for meet - SJSU vs UCD vs UCSC
Changed the xlsx files and parameters to update the demands of other schools. Added a conflict and player stats -- how much back to back games they have, and when their first and last games are.
</commit_message>
<xml_diff>
--- a/sjsu.xlsx
+++ b/sjsu.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="41">
   <si>
     <t>WS</t>
   </si>
@@ -22,109 +22,109 @@
     <t>Sankhya Gunda</t>
   </si>
   <si>
+    <t>Natalie Luong</t>
+  </si>
+  <si>
+    <t>Amber Li</t>
+  </si>
+  <si>
     <t>Sandara Cabagbag</t>
   </si>
   <si>
     <t>MD</t>
   </si>
   <si>
+    <t>Khang Nguyen</t>
+  </si>
+  <si>
+    <t>Tyler Yeh</t>
+  </si>
+  <si>
+    <t>Sean Hsieh</t>
+  </si>
+  <si>
+    <t>Benny Wen</t>
+  </si>
+  <si>
+    <t>Toan Le</t>
+  </si>
+  <si>
+    <t>Kyle Wong</t>
+  </si>
+  <si>
+    <t>Alex Nguyen</t>
+  </si>
+  <si>
+    <t>Alex Luong</t>
+  </si>
+  <si>
+    <t>Victor Tran</t>
+  </si>
+  <si>
+    <t>Cheng Huan Yu</t>
+  </si>
+  <si>
+    <t>Seong Kang Kwong</t>
+  </si>
+  <si>
+    <t>Logan Lei Chong</t>
+  </si>
+  <si>
+    <t>Khoa Tran</t>
+  </si>
+  <si>
+    <t>Khoa Nguyen</t>
+  </si>
+  <si>
+    <t>Paul Bishop</t>
+  </si>
+  <si>
+    <t>Parth Gopakumar</t>
+  </si>
+  <si>
+    <t>Jun Quan Yap</t>
+  </si>
+  <si>
+    <t>Kien Than</t>
+  </si>
+  <si>
+    <t>Benjamin Do</t>
+  </si>
+  <si>
+    <t>Juan David Liang</t>
+  </si>
+  <si>
+    <t>Ethan Phan</t>
+  </si>
+  <si>
+    <t>Kenneth Darla</t>
+  </si>
+  <si>
+    <t>WD</t>
+  </si>
+  <si>
+    <t>Emily Kung</t>
+  </si>
+  <si>
+    <t>Chelsea Lin</t>
+  </si>
+  <si>
+    <t>Niketana Thimma</t>
+  </si>
+  <si>
+    <t>Genevieve Le</t>
+  </si>
+  <si>
+    <t>Shani Chiu</t>
+  </si>
+  <si>
+    <t>MS</t>
+  </si>
+  <si>
     <t>Kelvin Chong</t>
   </si>
   <si>
     <t>Brandon Lee</t>
-  </si>
-  <si>
-    <t>Khang Nguyen</t>
-  </si>
-  <si>
-    <t>Tyler Yeh</t>
-  </si>
-  <si>
-    <t>Sean Hsieh</t>
-  </si>
-  <si>
-    <t>Benny Wen</t>
-  </si>
-  <si>
-    <t>Toan Le</t>
-  </si>
-  <si>
-    <t>Kyle Wong</t>
-  </si>
-  <si>
-    <t>Alex Nguyen</t>
-  </si>
-  <si>
-    <t>Alex Luong</t>
-  </si>
-  <si>
-    <t>Victor Tran</t>
-  </si>
-  <si>
-    <t>Cheng Huan Yu</t>
-  </si>
-  <si>
-    <t>Khoa Tran</t>
-  </si>
-  <si>
-    <t>Khoa Nguyen</t>
-  </si>
-  <si>
-    <t>Paul Bishop</t>
-  </si>
-  <si>
-    <t>Parth Gopakumar</t>
-  </si>
-  <si>
-    <t>Jun Quan Yap</t>
-  </si>
-  <si>
-    <t>Kien Than</t>
-  </si>
-  <si>
-    <t>Seong Kang Kwong</t>
-  </si>
-  <si>
-    <t>Logan Lei Chong</t>
-  </si>
-  <si>
-    <t>Benjamin Do</t>
-  </si>
-  <si>
-    <t>Juan David Liang</t>
-  </si>
-  <si>
-    <t>Ethan Phan</t>
-  </si>
-  <si>
-    <t>Kenneth Darla</t>
-  </si>
-  <si>
-    <t>WD</t>
-  </si>
-  <si>
-    <t>Amber Li</t>
-  </si>
-  <si>
-    <t>Emily Kung</t>
-  </si>
-  <si>
-    <t>Natalie Luong</t>
-  </si>
-  <si>
-    <t>Chelsea Lin</t>
-  </si>
-  <si>
-    <t>Niketana Thimma</t>
-  </si>
-  <si>
-    <t>Genevieve Le</t>
-  </si>
-  <si>
-    <t>Shani Chiu</t>
-  </si>
-  <si>
-    <t>MS</t>
   </si>
   <si>
     <t>Aditya Nagpal</t>
@@ -472,7 +472,7 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -506,7 +506,7 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -523,7 +523,7 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
@@ -540,7 +540,7 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
@@ -568,7 +568,7 @@
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
@@ -585,10 +585,10 @@
         <v>1.0</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
@@ -605,10 +605,10 @@
         <v>2.0</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -625,10 +625,10 @@
         <v>3.0</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -645,10 +645,10 @@
         <v>4.0</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -665,10 +665,10 @@
         <v>5.0</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -685,10 +685,10 @@
         <v>6.0</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -705,10 +705,10 @@
         <v>7.0</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -725,10 +725,10 @@
         <v>8.0</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -745,10 +745,10 @@
         <v>9.0</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -765,10 +765,10 @@
         <v>10.0</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
@@ -785,10 +785,10 @@
         <v>11.0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
@@ -805,10 +805,10 @@
         <v>12.0</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
@@ -821,9 +821,15 @@
       <c r="L22" s="1"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
+      <c r="A23" s="5">
+        <v>13.0</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -835,10 +841,9 @@
       <c r="L23" s="1"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A24" s="2"/>
+      <c r="B24" s="6"/>
+      <c r="C24" s="6"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -850,14 +855,9 @@
       <c r="L24" s="1"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>30</v>
+      <c r="A25" s="1"/>
+      <c r="B25" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
@@ -871,13 +871,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
@@ -891,13 +891,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -911,13 +911,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="2">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B28" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
@@ -931,13 +931,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B29" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>3</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
@@ -951,13 +951,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="2">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -971,13 +971,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>1</v>
+        <v>33</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -990,9 +990,15 @@
       <c r="L31" s="1"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
+      <c r="A32" s="2">
+        <v>7.0</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1005,9 +1011,8 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1019,11 +1024,9 @@
       <c r="L33" s="1"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>5</v>
+      <c r="A34" s="1"/>
+      <c r="B34" s="2" t="s">
+        <v>35</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -1037,90 +1040,99 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>12</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="2">
-        <v>5.0</v>
+        <v>4.0</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="2">
-        <v>6.0</v>
+        <v>5.0</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="2">
-        <v>7.0</v>
+        <v>6.0</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="2">
-        <v>8.0</v>
+        <v>7.0</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="2">
-        <v>9.0</v>
+        <v>8.0</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="2">
-        <v>10.0</v>
+        <v>9.0</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="2">
+        <v>10.0</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="2">
         <v>11.0</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B45" s="3" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="5">
-        <v>12.0</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1"/>
@@ -1146,7 +1158,7 @@
         <v>2.0</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>10</v>
@@ -1160,7 +1172,7 @@
         <v>25</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -1168,10 +1180,10 @@
         <v>4.0</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
@@ -1179,10 +1191,10 @@
         <v>5.0</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
@@ -1190,10 +1202,10 @@
         <v>6.0</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
@@ -1201,7 +1213,7 @@
         <v>7.0</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>8</v>
@@ -1212,7 +1224,7 @@
         <v>8.0</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>40</v>
@@ -1226,7 +1238,7 @@
         <v>28</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
@@ -2190,32 +2202,31 @@
     <row r="1015" ht="15.75" customHeight="1"/>
     <row r="1016" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="25">
+  <mergeCells count="24">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B7:C7"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B25:C25"/>
     <mergeCell ref="B34:C34"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
     <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B40:C40"/>
     <mergeCell ref="B41:C41"/>
     <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>